<commit_message>
Commit teste do projeto
</commit_message>
<xml_diff>
--- a/campanhas_lucro.xlsx
+++ b/campanhas_lucro.xlsx
@@ -485,22 +485,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>153.85</v>
+        <v>1171.85</v>
       </c>
       <c r="E2" t="n">
-        <v>13.76</v>
+        <v>15.66</v>
       </c>
       <c r="F2" t="n">
-        <v>70</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>5.09</v>
+        <v>5.9</v>
       </c>
       <c r="H2" t="n">
-        <v>56.24</v>
+        <v>76.74000000000001</v>
       </c>
       <c r="I2" t="n">
-        <v>928.0151295322523</v>
+        <v>1290.911656375089</v>
       </c>
     </row>
     <row r="3">
@@ -520,22 +520,22 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>158.32</v>
+        <v>799.17</v>
       </c>
       <c r="E3" t="n">
-        <v>28.03</v>
+        <v>40</v>
       </c>
       <c r="F3" t="n">
-        <v>60.16</v>
+        <v>107.12</v>
       </c>
       <c r="G3" t="n">
-        <v>2.15</v>
+        <v>2.68</v>
       </c>
       <c r="H3" t="n">
-        <v>32.13</v>
+        <v>67.12</v>
       </c>
       <c r="I3" t="n">
-        <v>600.6017498554635</v>
+        <v>903.3062832407608</v>
       </c>
     </row>
     <row r="4">
@@ -555,22 +555,22 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>136.21</v>
+        <v>592.29</v>
       </c>
       <c r="E4" t="n">
-        <v>30.95</v>
+        <v>41.46</v>
       </c>
       <c r="F4" t="n">
-        <v>61.4</v>
+        <v>81</v>
       </c>
       <c r="G4" t="n">
-        <v>1.98</v>
+        <v>1.95</v>
       </c>
       <c r="H4" t="n">
-        <v>30.45</v>
+        <v>39.54</v>
       </c>
       <c r="I4" t="n">
-        <v>555.365906725766</v>
+        <v>653.6360762714494</v>
       </c>
     </row>
     <row r="5">
@@ -590,22 +590,22 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>150</v>
+        <v>943.48</v>
       </c>
       <c r="E5" t="n">
-        <v>36.63</v>
+        <v>53.18</v>
       </c>
       <c r="F5" t="n">
-        <v>84.08</v>
+        <v>118.48</v>
       </c>
       <c r="G5" t="n">
-        <v>2.3</v>
+        <v>2.23</v>
       </c>
       <c r="H5" t="n">
-        <v>47.45</v>
+        <v>65.30000000000001</v>
       </c>
       <c r="I5" t="n">
-        <v>803.1674145857996</v>
+        <v>1044.792563999131</v>
       </c>
     </row>
     <row r="6">
@@ -625,22 +625,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>157.04</v>
+        <v>292.19</v>
       </c>
       <c r="E6" t="n">
-        <v>17.67</v>
+        <v>23.46</v>
       </c>
       <c r="F6" t="n">
         <v>28.32</v>
       </c>
       <c r="G6" t="n">
-        <v>1.6</v>
+        <v>1.21</v>
       </c>
       <c r="H6" t="n">
-        <v>10.65</v>
+        <v>4.859999999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>303.6413269829034</v>
+        <v>299.7302612716045</v>
       </c>
     </row>
     <row r="7">
@@ -660,19 +660,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>150</v>
+        <v>127.5</v>
       </c>
       <c r="E7" t="n">
-        <v>34.1</v>
+        <v>46.58</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>14.4</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="H7" t="n">
-        <v>-34.1</v>
+        <v>-32.18</v>
       </c>
     </row>
     <row r="8">
@@ -692,22 +692,22 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>154.43</v>
+        <v>820.6900000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>12.89</v>
+        <v>16.01</v>
       </c>
       <c r="F8" t="n">
-        <v>51.6</v>
+        <v>62.8</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>3.92</v>
       </c>
       <c r="H8" t="n">
-        <v>38.71</v>
+        <v>46.78999999999999</v>
       </c>
       <c r="I8" t="n">
-        <v>687.2879687801117</v>
+        <v>893.2844084153039</v>
       </c>
     </row>
     <row r="9">
@@ -727,22 +727,22 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>209</v>
+        <v>1938.46</v>
       </c>
       <c r="E9" t="n">
-        <v>24.08</v>
+        <v>59.73</v>
       </c>
       <c r="F9" t="n">
-        <v>122.2</v>
+        <v>205.56</v>
       </c>
       <c r="G9" t="n">
-        <v>5.07</v>
+        <v>3.44</v>
       </c>
       <c r="H9" t="n">
-        <v>98.12</v>
+        <v>145.83</v>
       </c>
       <c r="I9" t="n">
-        <v>1559.659361836853</v>
+        <v>2164.714382970801</v>
       </c>
     </row>
     <row r="10">
@@ -762,19 +762,22 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>150</v>
+        <v>439.45</v>
       </c>
       <c r="E10" t="n">
-        <v>27.94</v>
+        <v>40.33</v>
       </c>
       <c r="F10" t="n">
-        <v>20.8</v>
+        <v>127.48</v>
       </c>
       <c r="G10" t="n">
-        <v>0.74</v>
+        <v>3.16</v>
       </c>
       <c r="H10" t="n">
-        <v>-7.140000000000001</v>
+        <v>87.15000000000001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>574.6627098395754</v>
       </c>
     </row>
     <row r="11">
@@ -794,19 +797,22 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>157.49</v>
+        <v>167.5</v>
       </c>
       <c r="E11" t="n">
-        <v>19.61</v>
+        <v>31.41</v>
       </c>
       <c r="F11" t="n">
-        <v>20.32</v>
+        <v>49.12</v>
       </c>
       <c r="G11" t="n">
-        <v>1.04</v>
+        <v>1.56</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7100000000000009</v>
+        <v>17.71</v>
+      </c>
+      <c r="I11" t="n">
+        <v>194.9769603127812</v>
       </c>
     </row>
     <row r="12">
@@ -826,22 +832,22 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>150</v>
+        <v>684.15</v>
       </c>
       <c r="E12" t="n">
-        <v>19.2</v>
+        <v>23.07</v>
       </c>
       <c r="F12" t="n">
-        <v>53.6</v>
+        <v>68</v>
       </c>
       <c r="G12" t="n">
-        <v>2.79</v>
+        <v>2.95</v>
       </c>
       <c r="H12" t="n">
-        <v>34.40000000000001</v>
+        <v>44.93</v>
       </c>
       <c r="I12" t="n">
-        <v>623.5291688461857</v>
+        <v>753.8586294101219</v>
       </c>
     </row>
     <row r="13">
@@ -861,22 +867,22 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>153.81</v>
+        <v>177.17</v>
       </c>
       <c r="E13" t="n">
-        <v>18.32</v>
+        <v>25.64</v>
       </c>
       <c r="F13" t="n">
-        <v>19.6</v>
+        <v>44.88</v>
       </c>
       <c r="G13" t="n">
-        <v>1.07</v>
+        <v>1.75</v>
       </c>
       <c r="H13" t="n">
-        <v>1.280000000000001</v>
+        <v>19.24</v>
       </c>
       <c r="I13" t="n">
-        <v>171.429690003579</v>
+        <v>207.0207462686567</v>
       </c>
     </row>
     <row r="14">
@@ -896,19 +902,22 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>111.02</v>
+        <v>100</v>
       </c>
       <c r="E14" t="n">
-        <v>24.83</v>
+        <v>34.29</v>
       </c>
       <c r="F14" t="n">
-        <v>13.2</v>
+        <v>55.8</v>
       </c>
       <c r="G14" t="n">
-        <v>0.53</v>
+        <v>1.63</v>
       </c>
       <c r="H14" t="n">
-        <v>-11.63</v>
+        <v>21.51</v>
+      </c>
+      <c r="I14" t="n">
+        <v>133.3726378502498</v>
       </c>
     </row>
     <row r="15">
@@ -928,22 +937,22 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>156.03</v>
+        <v>326.62</v>
       </c>
       <c r="E15" t="n">
-        <v>24.6</v>
+        <v>38.58</v>
       </c>
       <c r="F15" t="n">
-        <v>38.4</v>
+        <v>46.4</v>
       </c>
       <c r="G15" t="n">
-        <v>1.56</v>
+        <v>1.2</v>
       </c>
       <c r="H15" t="n">
-        <v>13.8</v>
+        <v>7.82</v>
       </c>
       <c r="I15" t="n">
-        <v>345.9922828510861</v>
+        <v>338.7526837744748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>